<commit_message>
- Update Product Backlog & Sprint Backlog
</commit_message>
<xml_diff>
--- a/BackLog/ProductBacklog-Sample.xlsx
+++ b/BackLog/ProductBacklog-Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkingAtHuflit\24.25.S1\CNPMNC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\TLDH\Nam 3 - HK1\CNPMNC\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AD470-3D6D-4E16-A0BE-D4546490ABD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9813FFF4-1856-43E3-BAF9-FB22259E1891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="798" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="798" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Information" sheetId="7" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Product backlog" sheetId="1" r:id="rId3"/>
     <sheet name="Sprint backlog" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>I. Requirements</t>
   </si>
@@ -86,13 +97,103 @@
   </si>
   <si>
     <t>SPRINT BACKLOG</t>
+  </si>
+  <si>
+    <t>Thiết kế database</t>
+  </si>
+  <si>
+    <t>Thiết kế GUI của chức năng quản lý menu</t>
+  </si>
+  <si>
+    <t>Cao Thiên Bảo</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc Đương</t>
+  </si>
+  <si>
+    <t>Lê Ngô Phúc Khang</t>
+  </si>
+  <si>
+    <t>Trần Bảo Ngọc</t>
+  </si>
+  <si>
+    <t>bao2211</t>
+  </si>
+  <si>
+    <t>NguyenNgocDuong257</t>
+  </si>
+  <si>
+    <t>AMK0711</t>
+  </si>
+  <si>
+    <t>Dev Team</t>
+  </si>
+  <si>
+    <t>Đương</t>
+  </si>
+  <si>
+    <t>Lập trình chức năng hiển thị danh sách menu món ăn</t>
+  </si>
+  <si>
+    <t>Lập trình chức năng bộ lọc + tìm kiếm món ăn</t>
+  </si>
+  <si>
+    <t>Ngọc</t>
+  </si>
+  <si>
+    <t>Bảo</t>
+  </si>
+  <si>
+    <t>Khang</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Phần mềm </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Quản Lý Quán Ăn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> là một hệ thống hỗ trợ các nhà hàng/quán ăn trong việc tổ chức, quản
+lý và vận hành hiệu quả toàn bộ hoạt động kinh doanh từ khâu gọi món, chế biến, phục vụ, thu ngân
+cho đến kiểm kê kho nguyên liệu, tính lương nhân viên và tổng hợp báo cáo doanh thu.
+Hệ thống giúp kết nối thông suốt giữa các bộ phận: bếp, phục vụ, quản lý và chủ đầu tư, nhằm giảm
+thiểu sai sót, nâng cao chất lượng dịch vụ, đồng thời hỗ trợ ra quyết định nhanh chóng, chính xác
+thông qua các báo cáo phân tích.
+Ngoài ra, phần mềm còn hỗ trợ lưu trữ lịch sử hoạt động, thống kê hiệu suất làm việc nhân viên,
+đồng thời tích hợp phân quyền chặt chẽ để bảo mật dữ liệu theo từng vai trò cụ thể trong tổ chức.
+Phần mềm là công cụ cần thiết giúp các quán ăn, nhà hàng từ quy mô nhỏ đến vừa có thể chuyển đổi
+số hiệu quả, tiết kiệm chi phí vận hành, tăng tính chuyên nghiệp và cải thiện trải nghiệm khách
+hàng.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dev Team, Scrum Master</t>
+  </si>
+  <si>
+    <t>Dev Team, Product Owner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,6 +229,21 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="7">
@@ -168,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -224,17 +340,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -279,7 +384,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -292,15 +397,11 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -316,7 +417,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -326,47 +427,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,253 +895,255 @@
   <dimension ref="A2:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1048,103 +1159,141 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F10"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.265625" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" customWidth="1"/>
-    <col min="4" max="4" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="253" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="253" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="3" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="20"/>
+    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="18">
+        <v>45910</v>
+      </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="20"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="18">
+        <v>45910</v>
+      </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="20"/>
+    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="18">
+        <v>45910</v>
+      </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="18">
+        <v>45910</v>
+      </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="22"/>
+    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1160,183 +1309,207 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.265625" customWidth="1"/>
-    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="C7" s="14"/>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="14"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="14"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="13"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="13"/>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="13"/>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="13"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="14"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="13"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="14"/>
-    </row>
-    <row r="32" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="13"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1350,40 +1523,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:J6"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" customWidth="1"/>
-    <col min="8" max="8" width="13.3984375" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1393,46 +1566,46 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B3" s="11"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A4" s="19" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9">
@@ -1447,117 +1620,157 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="D7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="18">
+        <v>45910</v>
+      </c>
+      <c r="F7" s="18">
+        <v>45917</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+    <row r="8" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="18">
+        <v>45910</v>
+      </c>
+      <c r="F8" s="18">
+        <v>45917</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+    <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="D9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="18">
+        <v>45910</v>
+      </c>
+      <c r="F9" s="18">
+        <v>45917</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+    <row r="10" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="18">
+        <v>45910</v>
+      </c>
+      <c r="F10" s="18">
+        <v>45917</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
   </sheetData>

</xml_diff>